<commit_message>
Fix #13398 - [Bug] Fix export composition packaging report
</commit_message>
<xml_diff>
--- a/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/en/ExportCompositionPackaging.xlsx
+++ b/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/en/ExportCompositionPackaging.xlsx
@@ -8,12 +8,15 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Produits" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Products" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Composition" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Emballage" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Packaging" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Emballage!$B$3:$N$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Composition!$B$3:$O$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Packaging!$B$3:$R$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Products!$B$4:$EB$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Packaging!$D$3:$O$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="317">
   <si>
     <t xml:space="preserve">TYPE</t>
   </si>
@@ -843,16 +846,31 @@
     <t xml:space="preserve">bcpg:compoList</t>
   </si>
   <si>
-    <t xml:space="preserve">bcpg:compoListProduct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:compoListProduct_bcpg:erpCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:compoListProduct_bcpg:productHierarchy1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:compoListProduct_bcpg:productHierarchy2</t>
+    <t xml:space="preserve">AllLevel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entity|bcpg:erpCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entity|bcpg:code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:depthLevel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:compoListProduct|cm:name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:compoListProduct|bcpg:erpCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:compoListProduct|bcpg:code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:compoListProduct|bcpg:productHierarchy1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:compoListProduct|bcpg:productHierarchy2</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:compoListQtySubFormula</t>
@@ -873,12 +891,24 @@
     <t xml:space="preserve">Product</t>
   </si>
   <si>
+    <t xml:space="preserve">Product – ERP Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product – beCPG Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level</t>
+  </si>
+  <si>
     <t xml:space="preserve">Component</t>
   </si>
   <si>
     <t xml:space="preserve">Component – ERP Code</t>
   </si>
   <si>
+    <t xml:space="preserve">Component – beCPG Code</t>
+  </si>
+  <si>
     <t xml:space="preserve">Component – Family</t>
   </si>
   <si>
@@ -900,34 +930,25 @@
     <t xml:space="preserve">bcpg:packagingList</t>
   </si>
   <si>
-    <t xml:space="preserve">AllLevel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entity|cm:description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:depthLevel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:packagingListProduct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:packagingListProduct_bcpg:erpCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:packagingListProduct_cm:description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:packagingListProduct_bcpg:productHierarchy1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:packagingListProduct_bcpg:productHierarchy2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:packagingListProduct_pack:tare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:packagingListProduct_pack:tareUnit</t>
+    <t xml:space="preserve">bcpg:packagingListProduct|cm:name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:packagingListProduct|bcpg:erpCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:packagingListProduct|bcpg:code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:packagingListProduct|bcpg:productHierarchy1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:packagingListProduct|bcpg:productHierarchy2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:packagingListProduct|pack:tare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:packagingListProduct|pack:tareUnit</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:packagingListQty</t>
@@ -945,22 +966,13 @@
     <t xml:space="preserve">bcpg:packagingListIsMaster</t>
   </si>
   <si>
-    <t xml:space="preserve">Level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Packaging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Component – Description</t>
-  </si>
-  <si>
     <t xml:space="preserve">Component – Tare</t>
   </si>
   <si>
     <t xml:space="preserve">Component – Tare unit</t>
   </si>
   <si>
-    <t xml:space="preserve">Yield %</t>
+    <t xml:space="preserve">Loss %</t>
   </si>
   <si>
     <t xml:space="preserve">Packaging level</t>
@@ -976,7 +988,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1011,14 +1023,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="9"/>
-      <color rgb="FF2A00FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1076,7 +1080,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1090,10 +1094,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1112,7 +1112,7 @@
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF2A00FF"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
@@ -1173,6 +1173,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1181,11 +1189,11 @@
   </sheetPr>
   <dimension ref="A1:EB4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="DU1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="ED3" activeCellId="0" sqref="ED3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.34"/>
@@ -1722,7 +1730,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="60.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>134</v>
       </c>
@@ -2285,6 +2293,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B4:EB4"/>
   <mergeCells count="14">
     <mergeCell ref="B3:AI3"/>
     <mergeCell ref="AJ3:AM3"/>
@@ -2308,6 +2317,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2317,24 +2327,25 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="40.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="22.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="40.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="13.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="30.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2344,6 +2355,11 @@
       <c r="B1" s="1" t="s">
         <v>271</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="79" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -2353,31 +2369,43 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K2" s="4" t="s">
         <v>280</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2385,44 +2413,58 @@
         <v>134</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>289</v>
+      <c r="M3" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B3:O3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2432,30 +2474,28 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="35.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="50.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="43.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="31.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="34.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="24.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="24.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="17.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="35.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="43.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="31.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="34.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="24.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="24.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2463,127 +2503,133 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="D1" s="1"/>
+        <v>272</v>
+      </c>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="49.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>293</v>
+        <v>274</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>294</v>
+        <v>275</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>279</v>
+        <v>311</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>284</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>134</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>157</v>
+        <v>287</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>306</v>
+        <v>288</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>307</v>
+        <v>289</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>287</v>
+        <v>313</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>311</v>
-      </c>
       <c r="O3" s="3" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>288</v>
+        <v>316</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>297</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:N3"/>
+  <autoFilter ref="B3:R3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix #19537 - [Bug] Update export composition packaging excel files
</commit_message>
<xml_diff>
--- a/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/en/ExportCompositionPackaging.xlsx
+++ b/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/en/ExportCompositionPackaging.xlsx
@@ -8,12 +8,14 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Produits" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Products" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Composition" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Emballage" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Packaging" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Emballage!$B$3:$N$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Composition!$B$3:$O$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Packaging!$D$3:$O$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Products!$B$4:$EB$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,12 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="317">
   <si>
     <t xml:space="preserve">TYPE</t>
   </si>
   <si>
-    <t xml:space="preserve">bcpg:finishedProduct</t>
+    <t xml:space="preserve">bcpg:product</t>
   </si>
   <si>
     <t xml:space="preserve">COLUMNS</t>
@@ -843,16 +845,31 @@
     <t xml:space="preserve">bcpg:compoList</t>
   </si>
   <si>
-    <t xml:space="preserve">bcpg:compoListProduct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:compoListProduct_bcpg:erpCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:compoListProduct_bcpg:productHierarchy1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:compoListProduct_bcpg:productHierarchy2</t>
+    <t xml:space="preserve">AllLevel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entity|bcpg:erpCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entity|bcpg:code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:depthLevel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:compoListProduct|cm:name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:compoListProduct|bcpg:erpCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:compoListProduct|bcpg:code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:compoListProduct|bcpg:productHierarchy1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:compoListProduct|bcpg:productHierarchy2</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:compoListQtySubFormula</t>
@@ -873,12 +890,24 @@
     <t xml:space="preserve">Product</t>
   </si>
   <si>
+    <t xml:space="preserve">Product – ERP Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product – beCPG Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level</t>
+  </si>
+  <si>
     <t xml:space="preserve">Component</t>
   </si>
   <si>
     <t xml:space="preserve">Component – ERP Code</t>
   </si>
   <si>
+    <t xml:space="preserve">Component – beCPG Code</t>
+  </si>
+  <si>
     <t xml:space="preserve">Component – Family</t>
   </si>
   <si>
@@ -900,34 +929,25 @@
     <t xml:space="preserve">bcpg:packagingList</t>
   </si>
   <si>
-    <t xml:space="preserve">AllLevel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entity|cm:description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:depthLevel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:packagingListProduct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:packagingListProduct_bcpg:erpCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:packagingListProduct_cm:description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:packagingListProduct_bcpg:productHierarchy1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:packagingListProduct_bcpg:productHierarchy2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:packagingListProduct_pack:tare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:packagingListProduct_pack:tareUnit</t>
+    <t xml:space="preserve">bcpg:packagingListProduct|cm:name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:packagingListProduct|bcpg:erpCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:packagingListProduct|bcpg:code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:packagingListProduct|bcpg:productHierarchy1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:packagingListProduct|bcpg:productHierarchy2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:packagingListProduct|pack:tare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:packagingListProduct|pack:tareUnit</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:packagingListQty</t>
@@ -945,22 +965,13 @@
     <t xml:space="preserve">bcpg:packagingListIsMaster</t>
   </si>
   <si>
-    <t xml:space="preserve">Level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Packaging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Component – Description</t>
-  </si>
-  <si>
     <t xml:space="preserve">Component – Tare</t>
   </si>
   <si>
     <t xml:space="preserve">Component – Tare unit</t>
   </si>
   <si>
-    <t xml:space="preserve">Yield %</t>
+    <t xml:space="preserve">Loss %</t>
   </si>
   <si>
     <t xml:space="preserve">Packaging level</t>
@@ -976,7 +987,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1011,14 +1022,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="9"/>
-      <color rgb="FF2A00FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1076,7 +1079,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1093,10 +1096,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1106,13 +1105,29 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF004254"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF2A00FF"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
@@ -1173,6 +1188,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1181,11 +1204,11 @@
   </sheetPr>
   <dimension ref="A1:EB4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="DU1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="ED3" activeCellId="0" sqref="ED3"/>
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.34"/>
@@ -1722,7 +1745,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="60.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>134</v>
       </c>
@@ -2285,6 +2308,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B4:EB4"/>
   <mergeCells count="14">
     <mergeCell ref="B3:AI3"/>
     <mergeCell ref="AJ3:AM3"/>
@@ -2302,12 +2326,13 @@
     <mergeCell ref="DT3:EB3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2317,24 +2342,25 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="40.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="22.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="40.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="13.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="30.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2344,6 +2370,11 @@
       <c r="B1" s="1" t="s">
         <v>271</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="79" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -2353,31 +2384,43 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="K2" s="4" t="s">
         <v>280</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2385,44 +2428,58 @@
         <v>134</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>289</v>
+      <c r="M3" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B3:O3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2432,30 +2489,28 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="35.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="50.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="43.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="31.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="34.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="24.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="24.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="17.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="35.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="43.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="31.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="34.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="24.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="24.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2463,124 +2518,130 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="D1" s="1"/>
+        <v>272</v>
+      </c>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="49.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>293</v>
+        <v>274</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>294</v>
+        <v>275</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>279</v>
+        <v>311</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>284</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>134</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>157</v>
+        <v>287</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>306</v>
+        <v>288</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>307</v>
+        <v>289</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>287</v>
+        <v>313</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>311</v>
-      </c>
       <c r="O3" s="3" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>288</v>
+        <v>316</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>297</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:N3"/>
+  <autoFilter ref="D3:O3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>